<commit_message>
Now able to grab information by ISBN number and write it to the spreadsheet.
</commit_message>
<xml_diff>
--- a/BookDatabase.xlsx
+++ b/BookDatabase.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCF3F82-6799-46E8-AD1E-1B85FDEBCD68}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9110" windowWidth="23040" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Book Inventory" sheetId="1" r:id="rId1"/>
-    <sheet name="Check Out-In" sheetId="2" r:id="rId2"/>
+    <sheet name="Book Inventory" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Check Out-In" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+  <si>
+    <t>Book Title:</t>
+  </si>
+  <si>
+    <t>Book Author:</t>
+  </si>
+  <si>
+    <t>ISBN:</t>
+  </si>
   <si>
     <t>Total Quantity:</t>
   </si>
@@ -29,13 +32,13 @@
     <t>In Stock:</t>
   </si>
   <si>
-    <t>ISBN:</t>
-  </si>
-  <si>
-    <t>Book Title:</t>
-  </si>
-  <si>
-    <t>Book Author:</t>
+    <t>The Hunger Games</t>
+  </si>
+  <si>
+    <t>Suzanne Collins</t>
+  </si>
+  <si>
+    <t>0439023483</t>
   </si>
   <si>
     <t>Checked Out By:</t>
@@ -47,19 +50,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,24 +79,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -358,77 +353,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="14.1796875"/>
+    <col customWidth="1" max="2" min="2" width="16"/>
+    <col bestFit="1" customWidth="1" max="4" min="3" width="14.26953125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="8.453125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348BD665-3A5D-4014-B24C-E84AE11DB28A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="10.453125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="12.54296875"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="15.54296875"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed from Google database to wcat. Changed to store values as numbers over text.
</commit_message>
<xml_diff>
--- a/BookDatabase.xlsx
+++ b/BookDatabase.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helpdesk.STMHIGHSCHOOL\Documents\Python Scripts\RespireBookScanner\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36662667-9F62-4E23-810F-9060CCE50903}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9110" windowWidth="23040" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Book Inventory" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Check Out-In" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Book Inventory" sheetId="1" r:id="rId1"/>
+    <sheet name="Check Out-In" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Book Title:</t>
   </si>
@@ -30,6 +36,15 @@
   </si>
   <si>
     <t>In Stock:</t>
+  </si>
+  <si>
+    <t>Where The Wild Things Are</t>
+  </si>
+  <si>
+    <t>Maurice Sendak</t>
+  </si>
+  <si>
+    <t>0064431789</t>
   </si>
   <si>
     <t>The Hunger Games</t>
@@ -50,20 +65,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -79,15 +93,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -353,26 +376,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="14.1796875"/>
-    <col customWidth="1" max="2" min="2" width="16"/>
-    <col bestFit="1" customWidth="1" max="4" min="3" width="14.26953125"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="8.453125"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,7 +409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -399,55 +419,52 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="10.453125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="12.54296875"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="15.54296875"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="11"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,13 +475,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First fully working build +  check_in() support
</commit_message>
<xml_diff>
--- a/BookDatabase.xlsx
+++ b/BookDatabase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Book Title:</t>
   </si>
@@ -33,40 +33,28 @@
     <t>In Stock:</t>
   </si>
   <si>
-    <t>Where The Wild Things Are</t>
-  </si>
-  <si>
-    <t>Maurice Sendak</t>
+    <t>The Hunger Games</t>
+  </si>
+  <si>
+    <t>Suzanne Collins</t>
+  </si>
+  <si>
+    <t>0439023483</t>
+  </si>
+  <si>
+    <t>Wild Things Storytelling Kit</t>
+  </si>
+  <si>
+    <t>story and pictures by Maurice Sendak</t>
   </si>
   <si>
     <t>0064431789</t>
   </si>
   <si>
-    <t>The Hunger Games</t>
-  </si>
-  <si>
-    <t>Suzanne Collins</t>
-  </si>
-  <si>
-    <t>0439023483</t>
-  </si>
-  <si>
     <t>Checked Out By:</t>
   </si>
   <si>
     <t>Date/Time:</t>
-  </si>
-  <si>
-    <t>Wild Things Storytelling Kit</t>
-  </si>
-  <si>
-    <t>story and pictures by Maurice Sendak</t>
-  </si>
-  <si>
-    <t>Grayson Guarino</t>
-  </si>
-  <si>
-    <t>2018-06-01 13:57:17</t>
   </si>
 </sst>
 </file>
@@ -478,26 +466,26 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="3" s="2" spans="1:5">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -514,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E5" activeCellId="0" pane="topLeft" sqref="E5"/>
@@ -547,23 +535,8 @@
         <v>12</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
+    <row customHeight="1" ht="15" r="2" s="2" spans="1:5"/>
+    <row r="3" spans="1:5"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
- Removed a line that printed a list for testing
</commit_message>
<xml_diff>
--- a/BookDatabase.xlsx
+++ b/BookDatabase.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdogp\Google Drive\Haiti Library Scanner\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB62C1C3-3632-4AE2-8D27-0DD530B09E1A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Book Inventory" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Check Out-In" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Book Inventory" sheetId="1" r:id="rId1"/>
+    <sheet name="Check Out-In" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Book Title:</t>
   </si>
@@ -39,16 +44,25 @@
     <t>Suzanne Collins</t>
   </si>
   <si>
-    <t>0439023483</t>
-  </si>
-  <si>
-    <t>Wild Things Storytelling Kit</t>
-  </si>
-  <si>
-    <t>story and pictures by Maurice Sendak</t>
-  </si>
-  <si>
-    <t>0064431789</t>
+    <t>9780439023528</t>
+  </si>
+  <si>
+    <t>The Outsiders</t>
+  </si>
+  <si>
+    <t>S.E. Hinton</t>
+  </si>
+  <si>
+    <t>9780140385724</t>
+  </si>
+  <si>
+    <t>To Kill A Mockingbird</t>
+  </si>
+  <si>
+    <t>by Harper Lee</t>
+  </si>
+  <si>
+    <t>9780446310789</t>
   </si>
   <si>
     <t>Checked Out By:</t>
@@ -60,35 +74,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -103,33 +101,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -417,62 +408,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="25.57"/>
-    <col customWidth="1" max="2" min="2" style="1" width="15.15"/>
-    <col customWidth="1" max="3" min="3" style="1" width="10.99"/>
-    <col customWidth="1" max="4" min="4" style="1" width="14.28"/>
-    <col customWidth="1" max="5" min="5" style="1" width="8.42"/>
-    <col customWidth="1" max="1025" min="6" style="1" width="8.67"/>
+    <col min="1" max="1" width="25.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" style="1" customWidth="1"/>
+    <col min="6" max="1025" width="8.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="2" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>2</v>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3" s="2" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -482,64 +469,74 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E5" activeCellId="0" pane="topLeft" sqref="E5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="23.66"/>
-    <col customWidth="1" max="2" min="2" style="1" width="32.83"/>
-    <col customWidth="1" max="3" min="3" style="1" width="12.68"/>
-    <col customWidth="1" max="4" min="4" style="1" width="15.57"/>
-    <col customWidth="1" max="5" min="5" style="1" width="20.05"/>
-    <col customWidth="1" max="1025" min="6" style="1" width="8.67"/>
+    <col min="1" max="1" width="23.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="1" customWidth="1"/>
+    <col min="6" max="1025" width="8.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="2" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="2" spans="1:5"/>
-    <row r="3" spans="1:5"/>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>